<commit_message>
update with new MeSH table
</commit_message>
<xml_diff>
--- a/output/concepts.greece.xlsx
+++ b/output/concepts.greece.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -464,6 +464,31 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,64 +497,79 @@
         </is>
       </c>
       <c r="B2">
+        <v>38</v>
+      </c>
+      <c r="C2">
         <v>36</v>
       </c>
-      <c r="C2">
-        <v>33</v>
-      </c>
       <c r="D2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E2">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>59</v>
+      </c>
+      <c r="G2">
         <v>54</v>
       </c>
-      <c r="F2">
-        <v>53</v>
-      </c>
-      <c r="G2">
-        <v>52</v>
-      </c>
       <c r="H2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I2">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="J2">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="K2">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L2">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="M2">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="N2">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="O2">
+        <v>130</v>
+      </c>
+      <c r="P2">
+        <v>132</v>
+      </c>
+      <c r="Q2">
+        <v>130</v>
+      </c>
+      <c r="R2">
+        <v>107</v>
+      </c>
+      <c r="S2">
+        <v>130</v>
+      </c>
+      <c r="T2">
         <v>122</v>
       </c>
-      <c r="P2">
-        <v>122</v>
-      </c>
-      <c r="Q2">
-        <v>124</v>
-      </c>
-      <c r="R2">
-        <v>100</v>
-      </c>
-      <c r="S2">
-        <v>122</v>
-      </c>
-      <c r="T2">
-        <v>100</v>
-      </c>
       <c r="U2">
-        <v>31</v>
+        <v>152</v>
+      </c>
+      <c r="V2">
+        <v>195</v>
+      </c>
+      <c r="W2">
+        <v>249</v>
+      </c>
+      <c r="X2">
+        <v>244</v>
+      </c>
+      <c r="Y2">
+        <v>183</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -545,13 +585,13 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
       <c r="F3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -560,43 +600,58 @@
         <v>31</v>
       </c>
       <c r="I3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3">
         <v>33</v>
       </c>
       <c r="O3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P3">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Q3">
         <v>43</v>
       </c>
       <c r="R3">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="S3">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="T3">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="U3">
-        <v>16</v>
+        <v>65</v>
+      </c>
+      <c r="V3">
+        <v>80</v>
+      </c>
+      <c r="W3">
+        <v>110</v>
+      </c>
+      <c r="X3">
+        <v>114</v>
+      </c>
+      <c r="Y3">
+        <v>78</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -624,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -639,31 +694,46 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>5</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>10</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -673,7 +743,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -785,6 +855,31 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -793,64 +888,79 @@
         </is>
       </c>
       <c r="B2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E2">
+        <v>58</v>
+      </c>
+      <c r="F2">
         <v>54</v>
       </c>
-      <c r="F2">
-        <v>48</v>
-      </c>
       <c r="G2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I2">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="J2">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="K2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L2">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="M2">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="N2">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="O2">
+        <v>125</v>
+      </c>
+      <c r="P2">
+        <v>126</v>
+      </c>
+      <c r="Q2">
+        <v>124</v>
+      </c>
+      <c r="R2">
+        <v>102</v>
+      </c>
+      <c r="S2">
+        <v>128</v>
+      </c>
+      <c r="T2">
         <v>117</v>
       </c>
-      <c r="P2">
-        <v>118</v>
-      </c>
-      <c r="Q2">
-        <v>120</v>
-      </c>
-      <c r="R2">
-        <v>95</v>
-      </c>
-      <c r="S2">
-        <v>120</v>
-      </c>
-      <c r="T2">
-        <v>95</v>
-      </c>
       <c r="U2">
-        <v>31</v>
+        <v>151</v>
+      </c>
+      <c r="V2">
+        <v>191</v>
+      </c>
+      <c r="W2">
+        <v>247</v>
+      </c>
+      <c r="X2">
+        <v>244</v>
+      </c>
+      <c r="Y2">
+        <v>183</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -866,13 +976,13 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
       <c r="F3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -881,43 +991,58 @@
         <v>29</v>
       </c>
       <c r="I3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3">
         <v>31</v>
       </c>
       <c r="O3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P3">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Q3">
         <v>41</v>
       </c>
       <c r="R3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S3">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="T3">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="U3">
-        <v>16</v>
+        <v>65</v>
+      </c>
+      <c r="V3">
+        <v>80</v>
+      </c>
+      <c r="W3">
+        <v>111</v>
+      </c>
+      <c r="X3">
+        <v>114</v>
+      </c>
+      <c r="Y3">
+        <v>78</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -945,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -960,31 +1085,46 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>5</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>10</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>